<commit_message>
handles inheritance in plantuml
</commit_message>
<xml_diff>
--- a/examples/infrastructure/infrastructure.xlsx
+++ b/examples/infrastructure/infrastructure.xlsx
@@ -8,6 +8,8 @@
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Device" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Computer" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Harddisk" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -466,4 +468,86 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>os</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>osversion</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>location</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>vm</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>size</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>formfactor</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>rpm</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>computer</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
improves infrastructure example and adds test
</commit_message>
<xml_diff>
--- a/examples/infrastructure/infrastructure.xlsx
+++ b/examples/infrastructure/infrastructure.xlsx
@@ -10,6 +10,8 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Device" sheetId="1" state="visible" r:id="rId1"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Computer" sheetId="2" state="visible" r:id="rId2"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Harddisk" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Monitor" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Printer" sheetId="5" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -415,7 +417,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:Q1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -431,37 +433,82 @@
       </c>
       <c r="B1" t="inlineStr">
         <is>
+          <t>type</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
           <t>since</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="D1" t="inlineStr">
         <is>
           <t>until</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
+      <c r="E1" t="inlineStr">
         <is>
           <t>active</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
+      <c r="F1" t="inlineStr">
         <is>
           <t>purpose</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
+      <c r="G1" t="inlineStr">
         <is>
           <t>manufacturer</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
+      <c r="H1" t="inlineStr">
         <is>
           <t>model</t>
         </is>
       </c>
-      <c r="H1" t="inlineStr">
+      <c r="I1" t="inlineStr">
         <is>
           <t>serial</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>location</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>ip</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>mac</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>website</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>driver</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>support</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>comment</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>computer</t>
         </is>
       </c>
     </row>
@@ -476,7 +523,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -497,11 +544,6 @@
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>location</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
           <t>vm</t>
         </is>
       </c>
@@ -517,7 +559,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -541,13 +583,52 @@
           <t>rpm</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>computer</t>
-        </is>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>resolution</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>